<commit_message>
Completed model parameters table using revised models and lagged models
</commit_message>
<xml_diff>
--- a/tables/Model Parameters.xlsx
+++ b/tables/Model Parameters.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriellameltzer/Git/tropical_cyclones_educational_attainment_2022/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EFBBFF-3265-744B-8C97-7E01CBF557D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CE9184-A098-924F-A29E-376B752F58E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15560" yWindow="500" windowWidth="28040" windowHeight="16240" activeTab="1" xr2:uid="{09DAD223-5B37-144B-8D79-2569A973BF72}"/>
+    <workbookView xWindow="15140" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="2" xr2:uid="{09DAD223-5B37-144B-8D79-2569A973BF72}"/>
   </bookViews>
   <sheets>
     <sheet name="No EM" sheetId="1" r:id="rId1"/>
     <sheet name="EM Models" sheetId="2" r:id="rId2"/>
+    <sheet name="Revised" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="779">
   <si>
     <t>Storm Type</t>
   </si>
@@ -1993,13 +1994,394 @@
   </si>
   <si>
     <t>0.10 (-0.06, 0.25)</t>
+  </si>
+  <si>
+    <t>Normal/Lagged</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>-1.17 (-1.99, -0.35)</t>
+  </si>
+  <si>
+    <t>-2.02 (-2.19, -1.85)</t>
+  </si>
+  <si>
+    <t>-0.28 (-0.35, -0.21)</t>
+  </si>
+  <si>
+    <t>0.60 (0.13, 1.07)</t>
+  </si>
+  <si>
+    <t>0.13 (-0.02, 0.28)</t>
+  </si>
+  <si>
+    <t>0.31 (-0.02, 0.64)</t>
+  </si>
+  <si>
+    <t>-0.05 (-0.12, 0.02)</t>
+  </si>
+  <si>
+    <t>2.05 (1.72, 2.39)</t>
+  </si>
+  <si>
+    <t>-0.83 (-1.11, -0.54)</t>
+  </si>
+  <si>
+    <t>-0.29 (-0.56, -0.01)</t>
+  </si>
+  <si>
+    <t>0.05 (-0.25, 0.36)</t>
+  </si>
+  <si>
+    <t>0.19 (0.11, 0.27)</t>
+  </si>
+  <si>
+    <t>-0.01 (-0.25, 0.22)</t>
+  </si>
+  <si>
+    <t>-0.13 (-0.33, 0.06)</t>
+  </si>
+  <si>
+    <t>-0.15 (-0.26, -0.04)</t>
+  </si>
+  <si>
+    <t>-0.19 (-0.40, 0.00)</t>
+  </si>
+  <si>
+    <t>-0.09 (-0.21, 0.02)</t>
+  </si>
+  <si>
+    <t>0.05 (-0.01, 0.12)</t>
+  </si>
+  <si>
+    <t>0.01 (-0.07, 0.09)</t>
+  </si>
+  <si>
+    <t>0.00 (-0.15, 0.16)</t>
+  </si>
+  <si>
+    <t>-0.02 (-0.16, 0.10)</t>
+  </si>
+  <si>
+    <t>0.03 (-0.05, 0.12)</t>
+  </si>
+  <si>
+    <t>-1.70 (-2.41, -0.99)</t>
+  </si>
+  <si>
+    <t>-1.07 (-1.45, -0.68)</t>
+  </si>
+  <si>
+    <t>0.20 (0.07, 0.33)</t>
+  </si>
+  <si>
+    <t>0.87 (0.59, 1.16)</t>
+  </si>
+  <si>
+    <t>-0.57 (-0.63, -0.51)</t>
+  </si>
+  <si>
+    <t>1.74 (1.46, 2.01)</t>
+  </si>
+  <si>
+    <t>-0.08 (-0.31, 0.16)</t>
+  </si>
+  <si>
+    <t>0.10 (-0.13, 0.33)</t>
+  </si>
+  <si>
+    <t>0.07 (-0.19, 0.32)</t>
+  </si>
+  <si>
+    <t>-0.49 (-0.86, -0.12)</t>
+  </si>
+  <si>
+    <t>1.59 (1.17, 2.02)</t>
+  </si>
+  <si>
+    <t>-0.91 (-1.01, -0.82)</t>
+  </si>
+  <si>
+    <t>-1.70 (-1.79, -1.60)</t>
+  </si>
+  <si>
+    <t>0.00 (-0.03, 0.04)</t>
+  </si>
+  <si>
+    <t>-0.61 (-0.83, -0.39)</t>
+  </si>
+  <si>
+    <t>-0.29 (-0.33, -0.26)</t>
+  </si>
+  <si>
+    <t>1.59 (1.42, 1.75)</t>
+  </si>
+  <si>
+    <t>-0.42 (-0.56, -0.28)</t>
+  </si>
+  <si>
+    <t>-0.02 (-0.01, 0.00)</t>
+  </si>
+  <si>
+    <t>0.15 (0.03, 0.29)</t>
+  </si>
+  <si>
+    <t>-0.02 (-0.05, 0.00)</t>
+  </si>
+  <si>
+    <t>-0.06 (-0.10, -0.03)</t>
+  </si>
+  <si>
+    <t>0.10 (-0.01, 0.20)</t>
+  </si>
+  <si>
+    <t>-0.13 (-0.08, 0.02)</t>
+  </si>
+  <si>
+    <t>-0.01 (-0.03, 0.02)</t>
+  </si>
+  <si>
+    <t>0.12 (0.05, 0.19)</t>
+  </si>
+  <si>
+    <t>1.42 (1.06, 1.79)</t>
+  </si>
+  <si>
+    <t>-1.51 (-1.60, -1.43)</t>
+  </si>
+  <si>
+    <t>-1.89 (-1.97, -1.81)</t>
+  </si>
+  <si>
+    <t>-1.29 (-1.48, -1.10)</t>
+  </si>
+  <si>
+    <t>0.52 (0.41, 0.62)</t>
+  </si>
+  <si>
+    <t>-0.51 (-0.54, -0.49)</t>
+  </si>
+  <si>
+    <t>1.80 (1.66, 1.94)</t>
+  </si>
+  <si>
+    <t>-0.38 (-0.50, -0.25)</t>
+  </si>
+  <si>
+    <t>0.23 (0.10, 0.35)</t>
+  </si>
+  <si>
+    <t>0.07 (-0.06, 0.20)</t>
+  </si>
+  <si>
+    <t>Lagged</t>
+  </si>
+  <si>
+    <t>-1.45 (-2.38, -0.51)</t>
+  </si>
+  <si>
+    <t>1.78 (0.70, 2.86)</t>
+  </si>
+  <si>
+    <t>-0.96 (-1.14, -0.78)</t>
+  </si>
+  <si>
+    <t>-1.71 (-1.93, -1.48)</t>
+  </si>
+  <si>
+    <t>-0.45 (-0.53, -0.37)</t>
+  </si>
+  <si>
+    <t>0.66 (0.14, 1.19)</t>
+  </si>
+  <si>
+    <t>0.17 (0.00, 0.33)</t>
+  </si>
+  <si>
+    <t>-1.73 (-2.26, -1.20)</t>
+  </si>
+  <si>
+    <t>-0.49 (-0.59, -0.38)</t>
+  </si>
+  <si>
+    <t>1.64 (1.25, 2.04)</t>
+  </si>
+  <si>
+    <t>-0.76 (-1.11, -0.41)</t>
+  </si>
+  <si>
+    <t>0.04 (-0.29, 0.36)</t>
+  </si>
+  <si>
+    <t>-0.13 (-0.50, 0.25)</t>
+  </si>
+  <si>
+    <t>-2.01 (-2.83, -1.19)</t>
+  </si>
+  <si>
+    <t>1.80 (0.88, 2.72)</t>
+  </si>
+  <si>
+    <t>-1.67 (-1.82, -1.52)</t>
+  </si>
+  <si>
+    <t>-2.27 (-2.47, -2.07)</t>
+  </si>
+  <si>
+    <t>0.01 (-0.06, 0.08)</t>
+  </si>
+  <si>
+    <t>-1.61 (-2.04, -1.17)</t>
+  </si>
+  <si>
+    <t>0.25 (0.11, 0.39)</t>
+  </si>
+  <si>
+    <t>0.37 (-0.09, 0.82)</t>
+  </si>
+  <si>
+    <t>-0.97 (-1.06, -0.89)</t>
+  </si>
+  <si>
+    <t>1.47 (1.14, 1.80)</t>
+  </si>
+  <si>
+    <t>0.21 (-0.08, 0.49)</t>
+  </si>
+  <si>
+    <t>0.34 (0.07, 0.61)</t>
+  </si>
+  <si>
+    <t>-0.31 (-0.62, -0.01)</t>
+  </si>
+  <si>
+    <t>0.14 (0.02, 0.26)</t>
+  </si>
+  <si>
+    <t>-0.06 (-0.31, 0.16)</t>
+  </si>
+  <si>
+    <t>-0.11 (-0.31, 0.06)</t>
+  </si>
+  <si>
+    <t>-0.16 (-0.30, -0.04)</t>
+  </si>
+  <si>
+    <t>-0.13 (-0.36, 0.06)</t>
+  </si>
+  <si>
+    <t>0.03 (-0.10, 0.16)</t>
+  </si>
+  <si>
+    <t>0.11 (0.01, 0.21)</t>
+  </si>
+  <si>
+    <t>-0.04 (-0.18, 0.09)</t>
+  </si>
+  <si>
+    <t>-0.05 (-0.15, 0.05)</t>
+  </si>
+  <si>
+    <t>-0.01 (-0.15, 0.13)</t>
+  </si>
+  <si>
+    <t>-0.04 (-0.14, 0.05)</t>
+  </si>
+  <si>
+    <t>-1.69 (-1.79, -1.60)</t>
+  </si>
+  <si>
+    <t>0.94 (0.81, 1.06)</t>
+  </si>
+  <si>
+    <t>-0.57 (-0.71, -0.42)</t>
+  </si>
+  <si>
+    <t>0.15 (-0.01, 0.30)</t>
+  </si>
+  <si>
+    <t>-1.89 (-1.97, -1.80)</t>
+  </si>
+  <si>
+    <t>-1.29 (-1.49, -1.10)</t>
+  </si>
+  <si>
+    <t>1.81 (1.67, 1.95)</t>
+  </si>
+  <si>
+    <t>-0.38 (-0.51, -0.26)</t>
+  </si>
+  <si>
+    <t>0.23 (0.11, 0.35)</t>
+  </si>
+  <si>
+    <t>-0.01 (-0.01, 0.00)</t>
+  </si>
+  <si>
+    <t>-0.01 (-0.06, 0.05)</t>
+  </si>
+  <si>
+    <t>0.21 (0.07, 0.34)</t>
+  </si>
+  <si>
+    <t>0.01 (-0.01, 0.03)</t>
+  </si>
+  <si>
+    <t>0.00 (0.03, 0.02)</t>
+  </si>
+  <si>
+    <t>-0.06 (-0.09, -0.02)</t>
+  </si>
+  <si>
+    <t>0.06 (0.03, 0.10)</t>
+  </si>
+  <si>
+    <t>-0.05 (-0.10, -0.01)</t>
+  </si>
+  <si>
+    <t>-0.03 (-0.05, 0.00)</t>
+  </si>
+  <si>
+    <t>-0.04 (-0.06, -0.01)</t>
+  </si>
+  <si>
+    <t>-0.25 (-0.31, -0.18)</t>
+  </si>
+  <si>
+    <t>0.14 (0.06, 0.23)</t>
+  </si>
+  <si>
+    <t>-0.05 (-0.11, 0.01)</t>
+  </si>
+  <si>
+    <t>0.12 (0.01, 0.24)</t>
+  </si>
+  <si>
+    <t>0.07 (0.05, 0.10)</t>
+  </si>
+  <si>
+    <t>-0.03 (-0.06, 0.01)</t>
+  </si>
+  <si>
+    <t>0.00 (-0.05, 0.04)</t>
+  </si>
+  <si>
+    <t>-0.04 (-0.08, 0.00)</t>
+  </si>
+  <si>
+    <t>-0.11 (-0.17, -0.05)</t>
+  </si>
+  <si>
+    <t>0.15 (0.08, 0.22)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2009,6 +2391,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2062,31 +2452,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2403,9 +2789,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48181F9-BFED-A84B-8D42-DC69B76F3A0D}">
   <dimension ref="A1:V161"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H140" sqref="H140"/>
+    <sheetView topLeftCell="B1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E103" sqref="E103:E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2433,534 +2819,530 @@
     <col min="22" max="22" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="V2" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="N3" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="20" t="s">
+      <c r="Q3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="R3" t="s">
         <v>54</v>
       </c>
-      <c r="S3" s="14" t="s">
+      <c r="S3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="T3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="U3" t="s">
         <v>57</v>
       </c>
-      <c r="V3" s="14" t="s">
+      <c r="V3" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12" t="s">
+      <c r="E4" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E5" s="12" t="s">
+      <c r="E5" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E6" s="12" t="s">
+      <c r="E6" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E7" s="12" t="s">
+      <c r="E7" t="s">
         <v>93</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E8" s="12" t="s">
+      <c r="E8" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E9" s="12" t="s">
+      <c r="E9" t="s">
         <v>95</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E10" s="12" t="s">
+      <c r="E10" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E11" s="18" t="s">
+    <row r="11" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="10" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="7" t="s">
+      <c r="M12" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="N12" s="8" t="s">
+      <c r="N12" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O12" s="8" t="s">
+      <c r="O12" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="P12" s="6" t="s">
+      <c r="P12" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Q12" s="7" t="s">
+      <c r="Q12" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="R12" s="6" t="s">
+      <c r="R12" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="S12" s="8" t="s">
+      <c r="S12" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="T12" s="10" t="s">
+      <c r="T12" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="U12" s="6" t="s">
+      <c r="U12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="V12" s="6" t="s">
+      <c r="V12" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" t="s">
         <v>108</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="K13" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L13" s="14" t="s">
+      <c r="L13" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="M13" s="13" t="s">
+      <c r="M13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="N13" s="14" t="s">
+      <c r="N13" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O13" s="14" t="s">
+      <c r="O13" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="P13" s="12" t="s">
+      <c r="P13" t="s">
         <v>70</v>
       </c>
-      <c r="Q13" s="13" t="s">
+      <c r="Q13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="R13" s="16" t="s">
+      <c r="R13" t="s">
         <v>85</v>
       </c>
-      <c r="S13" s="14" t="s">
+      <c r="S13" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="T13" s="20" t="s">
+      <c r="T13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="U13" s="12" t="s">
+      <c r="U13" t="s">
         <v>88</v>
       </c>
-      <c r="V13" s="16" t="s">
+      <c r="V13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E14" s="12" t="s">
+      <c r="E14" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E15" s="12" t="s">
+      <c r="E15" t="s">
         <v>91</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E16" s="12" t="s">
+      <c r="E16" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E17" s="12" t="s">
+      <c r="E17" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E18" s="12" t="s">
+      <c r="E18" t="s">
         <v>94</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E19" s="12" t="s">
+      <c r="E19" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E20" s="12" t="s">
+      <c r="E20" t="s">
         <v>96</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E21" s="18" t="s">
+    <row r="21" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E21" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="K22" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="L22" s="8" t="s">
+      <c r="L22" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="M22" s="7" t="s">
+      <c r="M22" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="N22" s="11" t="s">
+      <c r="N22" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="O22" s="8" t="s">
+      <c r="O22" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="P22" s="8" t="s">
+      <c r="P22" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="Q22" s="7" t="s">
+      <c r="Q22" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="R22" s="7" t="s">
+      <c r="R22" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="S22" s="8" t="s">
+      <c r="S22" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="T22" s="7" t="s">
+      <c r="T22" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="U22" s="7" t="s">
+      <c r="U22" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="V22" s="8" t="s">
+      <c r="V22" s="7" t="s">
         <v>214</v>
       </c>
     </row>
@@ -2977,10 +3359,10 @@
       <c r="D23" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" t="s">
         <v>198</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -3248,76 +3630,76 @@
         <v>254</v>
       </c>
     </row>
-    <row r="51" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E51" s="17" t="s">
+    <row r="51" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E51" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="F51" s="23" t="s">
+      <c r="F51" s="12" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="52" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
+    <row r="52" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D52" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F52" s="11" t="s">
+      <c r="F52" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="G52" s="7" t="s">
+      <c r="G52" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="H52" s="8" t="s">
+      <c r="H52" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="I52" s="7" t="s">
+      <c r="I52" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="J52" s="7" t="s">
+      <c r="J52" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="K52" s="8" t="s">
+      <c r="K52" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="L52" s="8" t="s">
+      <c r="L52" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="M52" s="7" t="s">
+      <c r="M52" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="N52" s="9" t="s">
+      <c r="N52" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="O52" s="8" t="s">
+      <c r="O52" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="P52" s="7" t="s">
+      <c r="P52" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="Q52" s="7" t="s">
+      <c r="Q52" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="R52" s="9" t="s">
+      <c r="R52" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="S52" s="8" t="s">
+      <c r="S52" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="T52" s="7" t="s">
+      <c r="T52" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="U52" s="11" t="s">
+      <c r="U52" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="V52" s="9" t="s">
+      <c r="V52" s="8" t="s">
         <v>282</v>
       </c>
     </row>
@@ -3334,58 +3716,58 @@
       <c r="D53" t="s">
         <v>2</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" t="s">
         <v>44</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" t="s">
         <v>299</v>
       </c>
-      <c r="G53" s="13" t="s">
+      <c r="G53" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="H53" s="14" t="s">
+      <c r="H53" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="I53" s="13" t="s">
+      <c r="I53" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="J53" s="13" t="s">
+      <c r="J53" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="K53" s="14" t="s">
+      <c r="K53" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="L53" s="14" t="s">
+      <c r="L53" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="M53" s="13" t="s">
+      <c r="M53" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="N53" s="15" t="s">
+      <c r="N53" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="O53" s="14" t="s">
+      <c r="O53" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="P53" s="13" t="s">
+      <c r="P53" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="Q53" s="13" t="s">
+      <c r="Q53" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="R53" s="15" t="s">
+      <c r="R53" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="S53" s="14" t="s">
+      <c r="S53" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="T53" s="13" t="s">
+      <c r="T53" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="U53" s="12" t="s">
+      <c r="U53" t="s">
         <v>281</v>
       </c>
-      <c r="V53" s="15" t="s">
+      <c r="V53" s="1" t="s">
         <v>282</v>
       </c>
     </row>
@@ -3605,96 +3987,96 @@
         <v>249</v>
       </c>
     </row>
-    <row r="81" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E81" s="17" t="s">
+    <row r="81" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E81" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="F81" s="23" t="s">
+      <c r="F81" s="12" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="82" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="6" t="s">
+    <row r="82" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B82" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C82" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="D82" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F82" s="6" t="s">
+      <c r="F82" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="G82" s="10" t="s">
+      <c r="G82" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="H82" s="8" t="s">
+      <c r="H82" s="7" t="s">
         <v>392</v>
       </c>
-      <c r="I82" s="7" t="s">
+      <c r="I82" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="J82" s="7" t="s">
+      <c r="J82" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="K82" s="7" t="s">
+      <c r="K82" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="L82" s="10" t="s">
+      <c r="L82" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="M82" s="8" t="s">
+      <c r="M82" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="N82" s="6" t="s">
+      <c r="N82" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="O82" s="8" t="s">
+      <c r="O82" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="P82" s="8" t="s">
+      <c r="P82" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="Q82" s="6" t="s">
+      <c r="Q82" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="R82" s="7" t="s">
+      <c r="R82" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="S82" s="8" t="s">
+      <c r="S82" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="T82" s="7" t="s">
+      <c r="T82" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="U82" s="10" t="s">
+      <c r="U82" s="8" t="s">
         <v>405</v>
       </c>
-      <c r="V82" s="8" t="s">
+      <c r="V82" s="7" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A83" s="16" t="s">
+      <c r="A83" t="s">
         <v>389</v>
       </c>
-      <c r="B83" s="16" t="s">
+      <c r="B83" t="s">
         <v>20</v>
       </c>
-      <c r="C83" s="16" t="s">
+      <c r="C83" t="s">
         <v>23</v>
       </c>
-      <c r="D83" s="16" t="s">
+      <c r="D83" t="s">
         <v>2</v>
       </c>
-      <c r="E83" s="16" t="s">
+      <c r="E83" t="s">
         <v>44</v>
       </c>
-      <c r="F83" s="12" t="s">
+      <c r="F83" t="s">
         <v>446</v>
       </c>
       <c r="G83" s="2" t="s">
@@ -3747,155 +4129,151 @@
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A84" s="12"/>
-      <c r="B84" s="12"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12" t="s">
+      <c r="E84" t="s">
         <v>90</v>
       </c>
-      <c r="F84" s="12" t="s">
+      <c r="F84" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E85" s="12" t="s">
+      <c r="E85" t="s">
         <v>91</v>
       </c>
-      <c r="F85" s="14" t="s">
+      <c r="F85" s="3" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E86" s="12" t="s">
+      <c r="E86" t="s">
         <v>92</v>
       </c>
-      <c r="F86" s="12" t="s">
+      <c r="F86" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E87" s="12" t="s">
+      <c r="E87" t="s">
         <v>93</v>
       </c>
-      <c r="F87" s="12" t="s">
+      <c r="F87" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E88" s="12" t="s">
+      <c r="E88" t="s">
         <v>94</v>
       </c>
-      <c r="F88" s="15" t="s">
+      <c r="F88" s="1" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E89" s="12" t="s">
+      <c r="E89" t="s">
         <v>95</v>
       </c>
-      <c r="F89" s="12" t="s">
+      <c r="F89" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E90" s="12" t="s">
+      <c r="E90" t="s">
         <v>96</v>
       </c>
-      <c r="F90" s="12" t="s">
+      <c r="F90" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="91" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E91" s="18" t="s">
+    <row r="91" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E91" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F91" s="22" t="s">
+      <c r="F91" s="11" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="92" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="17" t="s">
+    <row r="92" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="B92" s="17" t="s">
+      <c r="B92" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C92" s="17" t="s">
+      <c r="C92" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D92" s="17" t="s">
+      <c r="D92" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F92" s="17" t="s">
+      <c r="F92" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="G92" s="22" t="s">
+      <c r="G92" s="11" t="s">
         <v>421</v>
       </c>
-      <c r="H92" s="23" t="s">
+      <c r="H92" s="12" t="s">
         <v>422</v>
       </c>
-      <c r="I92" s="22" t="s">
+      <c r="I92" s="11" t="s">
         <v>423</v>
       </c>
-      <c r="J92" s="22" t="s">
+      <c r="J92" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="K92" s="23" t="s">
+      <c r="K92" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="L92" s="23" t="s">
+      <c r="L92" s="12" t="s">
         <v>425</v>
       </c>
-      <c r="M92" s="22" t="s">
+      <c r="M92" s="11" t="s">
         <v>426</v>
       </c>
-      <c r="N92" s="23" t="s">
+      <c r="N92" s="12" t="s">
         <v>427</v>
       </c>
-      <c r="O92" s="23" t="s">
+      <c r="O92" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="P92" s="22" t="s">
+      <c r="P92" s="11" t="s">
         <v>428</v>
       </c>
-      <c r="Q92" s="22" t="s">
+      <c r="Q92" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="R92" s="21" t="s">
+      <c r="R92" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="S92" s="23" t="s">
+      <c r="S92" s="12" t="s">
         <v>431</v>
       </c>
-      <c r="T92" s="22" t="s">
+      <c r="T92" s="11" t="s">
         <v>432</v>
       </c>
-      <c r="U92" s="22" t="s">
+      <c r="U92" s="11" t="s">
         <v>433</v>
       </c>
-      <c r="V92" s="17" t="s">
+      <c r="V92" s="9" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A93" s="12" t="s">
+      <c r="A93" t="s">
         <v>389</v>
       </c>
-      <c r="B93" s="12" t="s">
+      <c r="B93" t="s">
         <v>20</v>
       </c>
-      <c r="C93" s="12" t="s">
+      <c r="C93" t="s">
         <v>59</v>
       </c>
-      <c r="D93" s="12" t="s">
+      <c r="D93" t="s">
         <v>2</v>
       </c>
-      <c r="E93" s="12" t="s">
+      <c r="E93" t="s">
         <v>44</v>
       </c>
-      <c r="F93" s="12" t="s">
+      <c r="F93" t="s">
         <v>292</v>
       </c>
       <c r="G93" s="2" t="s">
@@ -3948,131 +4326,131 @@
       </c>
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E94" s="12" t="s">
+      <c r="E94" t="s">
         <v>90</v>
       </c>
-      <c r="F94" s="12" t="s">
+      <c r="F94" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="95" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E95" s="12" t="s">
+      <c r="E95" t="s">
         <v>91</v>
       </c>
-      <c r="F95" s="14" t="s">
+      <c r="F95" s="3" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E96" s="12" t="s">
+      <c r="E96" t="s">
         <v>92</v>
       </c>
-      <c r="F96" s="14" t="s">
+      <c r="F96" s="3" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="97" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E97" s="12" t="s">
+      <c r="E97" t="s">
         <v>93</v>
       </c>
-      <c r="F97" s="12" t="s">
+      <c r="F97" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="98" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E98" s="12" t="s">
+      <c r="E98" t="s">
         <v>94</v>
       </c>
-      <c r="F98" s="15" t="s">
+      <c r="F98" s="1" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="99" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E99" s="12" t="s">
+      <c r="E99" t="s">
         <v>95</v>
       </c>
-      <c r="F99" s="12" t="s">
+      <c r="F99" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="100" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="E100" s="12" t="s">
+      <c r="E100" t="s">
         <v>96</v>
       </c>
-      <c r="F100" s="12" t="s">
+      <c r="F100" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="101" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E101" s="18" t="s">
+    <row r="101" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E101" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F101" s="22" t="s">
+      <c r="F101" s="11" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="102" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="6" t="s">
+    <row r="102" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="B102" s="6" t="s">
+      <c r="B102" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C102" s="6" t="s">
+      <c r="C102" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D102" s="6" t="s">
+      <c r="D102" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F102" s="6" t="s">
+      <c r="F102" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="G102" s="10" t="s">
+      <c r="G102" s="8" t="s">
         <v>532</v>
       </c>
-      <c r="H102" s="8" t="s">
+      <c r="H102" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="I102" s="7" t="s">
+      <c r="I102" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="J102" s="7" t="s">
+      <c r="J102" s="6" t="s">
         <v>535</v>
       </c>
-      <c r="K102" s="8" t="s">
+      <c r="K102" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="L102" s="8" t="s">
+      <c r="L102" s="7" t="s">
         <v>536</v>
       </c>
-      <c r="M102" s="7" t="s">
+      <c r="M102" s="6" t="s">
         <v>537</v>
       </c>
-      <c r="N102" s="6" t="s">
+      <c r="N102" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="O102" s="8" t="s">
+      <c r="O102" s="7" t="s">
         <v>538</v>
       </c>
-      <c r="P102" s="8" t="s">
+      <c r="P102" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="Q102" s="7" t="s">
+      <c r="Q102" s="6" t="s">
         <v>539</v>
       </c>
-      <c r="R102" s="7" t="s">
+      <c r="R102" s="6" t="s">
         <v>540</v>
       </c>
-      <c r="S102" s="8" t="s">
+      <c r="S102" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="T102" s="7" t="s">
+      <c r="T102" s="6" t="s">
         <v>542</v>
       </c>
-      <c r="U102" s="7" t="s">
+      <c r="U102" s="6" t="s">
         <v>543</v>
       </c>
-      <c r="V102" s="8" t="s">
+      <c r="V102" s="7" t="s">
         <v>544</v>
       </c>
     </row>
@@ -4089,10 +4467,10 @@
       <c r="D103" t="s">
         <v>2</v>
       </c>
-      <c r="E103" s="12" t="s">
+      <c r="E103" t="s">
         <v>44</v>
       </c>
-      <c r="F103" s="12" t="s">
+      <c r="F103" t="s">
         <v>266</v>
       </c>
       <c r="G103" s="1" t="s">
@@ -4360,78 +4738,78 @@
         <v>254</v>
       </c>
     </row>
-    <row r="131" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E131" s="17" t="s">
+    <row r="131" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E131" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="F131" s="23" t="s">
+      <c r="F131" s="12" t="s">
         <v>582</v>
       </c>
       <c r="G131"/>
       <c r="H131"/>
     </row>
-    <row r="132" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="6" t="s">
+    <row r="132" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="B132" s="6" t="s">
+      <c r="B132" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C132" s="6" t="s">
+      <c r="C132" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D132" s="6" t="s">
+      <c r="D132" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F132" s="6" t="s">
+      <c r="F132" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="G132" s="7" t="s">
+      <c r="G132" s="6" t="s">
         <v>556</v>
       </c>
-      <c r="H132" s="8" t="s">
+      <c r="H132" s="7" t="s">
         <v>557</v>
       </c>
-      <c r="I132" s="7" t="s">
+      <c r="I132" s="6" t="s">
         <v>558</v>
       </c>
-      <c r="J132" s="7" t="s">
+      <c r="J132" s="6" t="s">
         <v>559</v>
       </c>
-      <c r="K132" s="8" t="s">
+      <c r="K132" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="L132" s="8" t="s">
+      <c r="L132" s="7" t="s">
         <v>561</v>
       </c>
-      <c r="M132" s="7" t="s">
+      <c r="M132" s="6" t="s">
         <v>562</v>
       </c>
-      <c r="N132" s="7" t="s">
+      <c r="N132" s="6" t="s">
         <v>563</v>
       </c>
-      <c r="O132" s="8" t="s">
+      <c r="O132" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="P132" s="7" t="s">
+      <c r="P132" s="6" t="s">
         <v>564</v>
       </c>
-      <c r="Q132" s="7" t="s">
+      <c r="Q132" s="6" t="s">
         <v>565</v>
       </c>
-      <c r="R132" s="7" t="s">
+      <c r="R132" s="6" t="s">
         <v>566</v>
       </c>
-      <c r="S132" s="8" t="s">
+      <c r="S132" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="T132" s="7" t="s">
+      <c r="T132" s="6" t="s">
         <v>568</v>
       </c>
-      <c r="U132" s="7" t="s">
+      <c r="U132" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="V132" s="6" t="s">
+      <c r="V132" s="5" t="s">
         <v>570</v>
       </c>
     </row>
@@ -4448,7 +4826,7 @@
       <c r="D133" t="s">
         <v>2</v>
       </c>
-      <c r="E133" s="12" t="s">
+      <c r="E133" t="s">
         <v>44</v>
       </c>
       <c r="F133" t="s">
@@ -4499,7 +4877,7 @@
       <c r="U133" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="V133" s="4" t="s">
+      <c r="V133" s="1" t="s">
         <v>570</v>
       </c>
     </row>
@@ -4719,11 +5097,11 @@
         <v>249</v>
       </c>
     </row>
-    <row r="161" spans="5:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E161" s="17" t="s">
+    <row r="161" spans="5:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E161" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="F161" s="23" t="s">
+      <c r="F161" s="12" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4736,7 +5114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150A1CEB-6F12-7C40-A4DB-09C50B02073A}">
   <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
+    <sheetView zoomScale="171" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
     </sheetView>
@@ -4765,71 +5143,71 @@
     <col min="22" max="22" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4889,11 +5267,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E3" s="17" t="s">
+    <row r="3" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="10" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4953,69 +5331,69 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E5" s="17" t="s">
+    <row r="5" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E5" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="10" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" t="s">
         <v>146</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" t="s">
         <v>147</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="O6" s="3" t="s">
         <v>158</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E7" s="18" t="s">
+    <row r="7" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E7" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="9" t="s">
         <v>150</v>
       </c>
     </row>
@@ -5032,48 +5410,48 @@
       <c r="D8" t="s">
         <v>146</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" t="s">
         <v>147</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="M8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="O8" s="14" t="s">
+      <c r="O8" s="3" t="s">
         <v>168</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E9" s="18" t="s">
+    <row r="9" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E9" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="9" t="s">
         <v>161</v>
       </c>
     </row>
@@ -5090,67 +5468,66 @@
       <c r="D10" t="s">
         <v>169</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" t="s">
         <v>170</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" t="s">
         <v>172</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="M10" s="14" t="s">
+      <c r="M10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N10" s="12" t="s">
+      <c r="N10" t="s">
         <v>35</v>
       </c>
-      <c r="O10" s="15"/>
-      <c r="P10" s="14" t="s">
+      <c r="O10" s="1"/>
+      <c r="P10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Q10" s="15" t="s">
+      <c r="Q10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R10" s="15" t="s">
+      <c r="R10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S10" s="14" t="s">
+      <c r="S10" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="T10" s="13" t="s">
+      <c r="T10" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="U10" s="12" t="s">
+      <c r="U10" t="s">
         <v>180</v>
       </c>
-      <c r="V10" s="14" t="s">
+      <c r="V10" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E11" s="18" t="s">
+    <row r="11" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="J11" s="18"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -5165,34 +5542,34 @@
       <c r="D12" t="s">
         <v>169</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" t="s">
         <v>170</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" t="s">
         <v>182</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="K12" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="L12" s="14" t="s">
+      <c r="L12" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="M12" s="13" t="s">
+      <c r="M12" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="N12" s="14" t="s">
+      <c r="N12" s="3" t="s">
         <v>191</v>
       </c>
       <c r="P12" t="s">
@@ -5217,11 +5594,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E13" s="18" t="s">
+    <row r="13" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E13" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="10" t="s">
         <v>183</v>
       </c>
     </row>
@@ -5238,10 +5615,10 @@
       <c r="D14" t="s">
         <v>116</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" t="s">
         <v>309</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="3" t="s">
         <v>311</v>
       </c>
       <c r="K14" t="s">
@@ -5281,11 +5658,11 @@
         <v>323</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E15" s="18" t="s">
+    <row r="15" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E15" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="12" t="s">
         <v>312</v>
       </c>
     </row>
@@ -5302,10 +5679,10 @@
       <c r="D16" t="s">
         <v>116</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" t="s">
         <v>309</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="3" t="s">
         <v>324</v>
       </c>
       <c r="K16" s="3" t="s">
@@ -5345,11 +5722,11 @@
         <v>333</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E17" s="18" t="s">
+    <row r="17" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="9" t="s">
         <v>286</v>
       </c>
     </row>
@@ -5366,48 +5743,48 @@
       <c r="D18" t="s">
         <v>146</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" t="s">
         <v>334</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="J18" s="13" t="s">
+      <c r="J18" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="K18" t="s">
         <v>341</v>
       </c>
-      <c r="L18" s="14" t="s">
+      <c r="L18" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="M18" s="13" t="s">
+      <c r="M18" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="N18" s="12" t="s">
+      <c r="N18" t="s">
         <v>344</v>
       </c>
-      <c r="O18" s="14" t="s">
+      <c r="O18" s="3" t="s">
         <v>345</v>
       </c>
       <c r="Q18" s="2" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="19" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E19" s="18" t="s">
+    <row r="19" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E19" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="9" t="s">
         <v>337</v>
       </c>
     </row>
@@ -5424,48 +5801,48 @@
       <c r="D20" t="s">
         <v>146</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" t="s">
         <v>334</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" t="s">
         <v>286</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="L20" s="14" t="s">
+      <c r="L20" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="M20" s="13" t="s">
+      <c r="M20" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="N20" s="12" t="s">
+      <c r="N20" t="s">
         <v>24</v>
       </c>
-      <c r="O20" s="14" t="s">
+      <c r="O20" s="3" t="s">
         <v>354</v>
       </c>
       <c r="Q20" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="21" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E21" s="18" t="s">
+    <row r="21" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E21" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="12" t="s">
         <v>347</v>
       </c>
     </row>
@@ -5482,34 +5859,34 @@
       <c r="D22" t="s">
         <v>169</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" t="s">
         <v>357</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" t="s">
         <v>359</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="I22" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="K22" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="L22" s="14" t="s">
+      <c r="L22" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="M22" s="13" t="s">
+      <c r="M22" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="N22" s="12" t="s">
+      <c r="N22" t="s">
         <v>368</v>
       </c>
       <c r="P22" s="3" t="s">
@@ -5534,11 +5911,11 @@
         <v>375</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E23" s="18" t="s">
+    <row r="23" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E23" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="11" t="s">
         <v>360</v>
       </c>
     </row>
@@ -5555,34 +5932,34 @@
       <c r="D24" t="s">
         <v>169</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" t="s">
         <v>357</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" t="s">
         <v>376</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="K24" s="14" t="s">
+      <c r="K24" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="L24" s="14" t="s">
+      <c r="L24" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="M24" s="13" t="s">
+      <c r="M24" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="N24" s="15" t="s">
+      <c r="N24" s="1" t="s">
         <v>383</v>
       </c>
       <c r="P24" s="2" t="s">
@@ -5607,11 +5984,11 @@
         <v>388</v>
       </c>
     </row>
-    <row r="25" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E25" s="18" t="s">
+    <row r="25" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E25" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="11" t="s">
         <v>296</v>
       </c>
     </row>
@@ -5671,11 +6048,11 @@
         <v>472</v>
       </c>
     </row>
-    <row r="27" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E27" s="17" t="s">
+    <row r="27" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E27" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="10" t="s">
         <v>460</v>
       </c>
     </row>
@@ -5735,66 +6112,66 @@
         <v>482</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E29" s="17" t="s">
+    <row r="29" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E29" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="F29" s="21" t="s">
+      <c r="F29" s="10" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
+      <c r="A30" t="s">
         <v>389</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" t="s">
         <v>146</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" t="s">
         <v>147</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="H30" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="I30" s="13" t="s">
+      <c r="I30" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="J30" s="13" t="s">
+      <c r="J30" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="K30" s="13" t="s">
+      <c r="K30" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="L30" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="M30" s="14" t="s">
+      <c r="M30" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="N30" s="14" t="s">
+      <c r="N30" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="O30" s="14" t="s">
+      <c r="O30" s="3" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="31" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E31" s="18" t="s">
+    <row r="31" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E31" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="9" t="s">
         <v>484</v>
       </c>
     </row>
@@ -5811,45 +6188,45 @@
       <c r="D32" t="s">
         <v>146</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" t="s">
         <v>147</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="H32" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="I32" s="13" t="s">
+      <c r="I32" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="J32" s="13" t="s">
+      <c r="J32" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="K32" s="14" t="s">
+      <c r="K32" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="L32" s="14" t="s">
+      <c r="L32" s="3" t="s">
         <v>498</v>
       </c>
-      <c r="M32" s="13" t="s">
+      <c r="M32" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="N32" s="14" t="s">
+      <c r="N32" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="O32" s="14" t="s">
+      <c r="O32" s="3" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="33" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E33" s="18" t="s">
+    <row r="33" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E33" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F33" s="23" t="s">
+      <c r="F33" s="12" t="s">
         <v>494</v>
       </c>
     </row>
@@ -5866,34 +6243,34 @@
       <c r="D34" t="s">
         <v>169</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" t="s">
         <v>170</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="H34" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="I34" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="J34" s="13" t="s">
+      <c r="J34" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="K34" s="13" t="s">
+      <c r="K34" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="L34" s="15" t="s">
+      <c r="L34" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="M34" s="14" t="s">
+      <c r="M34" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="N34" s="12" t="s">
+      <c r="N34" t="s">
         <v>511</v>
       </c>
       <c r="P34" s="3" t="s">
@@ -5918,11 +6295,11 @@
         <v>518</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E35" s="18" t="s">
+    <row r="35" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E35" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="F35" s="9" t="s">
         <v>503</v>
       </c>
     </row>
@@ -5939,34 +6316,34 @@
       <c r="D36" t="s">
         <v>169</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" t="s">
         <v>170</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" t="s">
         <v>519</v>
       </c>
-      <c r="G36" s="13" t="s">
+      <c r="G36" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="H36" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="I36" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="J36" s="13" t="s">
+      <c r="J36" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="K36" s="14" t="s">
+      <c r="K36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L36" s="14" t="s">
+      <c r="L36" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="M36" s="13" t="s">
+      <c r="M36" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="N36" s="14" t="s">
+      <c r="N36" s="3" t="s">
         <v>526</v>
       </c>
       <c r="P36" s="2" t="s">
@@ -5991,11 +6368,11 @@
         <v>531</v>
       </c>
     </row>
-    <row r="37" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E37" s="18" t="s">
+    <row r="37" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E37" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="F37" s="21" t="s">
+      <c r="F37" s="10" t="s">
         <v>520</v>
       </c>
     </row>
@@ -6012,7 +6389,7 @@
       <c r="D38" t="s">
         <v>116</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" t="s">
         <v>309</v>
       </c>
       <c r="F38" s="3" t="s">
@@ -6055,11 +6432,11 @@
         <v>603</v>
       </c>
     </row>
-    <row r="39" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E39" s="18" t="s">
+    <row r="39" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E39" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="F39" s="23" t="s">
+      <c r="F39" s="12" t="s">
         <v>312</v>
       </c>
     </row>
@@ -6076,10 +6453,10 @@
       <c r="D40" t="s">
         <v>116</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" t="s">
         <v>309</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="3" t="s">
         <v>324</v>
       </c>
       <c r="K40" s="3" t="s">
@@ -6119,14 +6496,13 @@
         <v>611</v>
       </c>
     </row>
-    <row r="41" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E41" s="18" t="s">
+    <row r="41" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E41" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="F41" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="V41" s="18"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -6141,19 +6517,19 @@
       <c r="D42" t="s">
         <v>146</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" t="s">
         <v>334</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="G42" s="15" t="s">
+      <c r="G42" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="H42" s="14" t="s">
+      <c r="H42" s="3" t="s">
         <v>615</v>
       </c>
-      <c r="I42" s="13" t="s">
+      <c r="I42" s="2" t="s">
         <v>534</v>
       </c>
       <c r="J42" s="2" t="s">
@@ -6178,11 +6554,11 @@
         <v>621</v>
       </c>
     </row>
-    <row r="43" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E43" s="18" t="s">
+    <row r="43" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E43" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="F43" s="19" t="s">
+      <c r="F43" s="10" t="s">
         <v>336</v>
       </c>
     </row>
@@ -6199,48 +6575,48 @@
       <c r="D44" t="s">
         <v>146</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" t="s">
         <v>334</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="F44" t="s">
         <v>337</v>
       </c>
-      <c r="G44" s="13" t="s">
+      <c r="G44" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="H44" s="14" t="s">
+      <c r="H44" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="I44" s="13" t="s">
+      <c r="I44" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="J44" s="13" t="s">
+      <c r="J44" s="2" t="s">
         <v>624</v>
       </c>
-      <c r="K44" s="14" t="s">
+      <c r="K44" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="L44" s="14" t="s">
+      <c r="L44" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="M44" s="13" t="s">
+      <c r="M44" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="N44" s="15" t="s">
+      <c r="N44" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="O44" s="14" t="s">
+      <c r="O44" s="3" t="s">
         <v>628</v>
       </c>
       <c r="Q44" s="2" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="45" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E45" s="18" t="s">
+    <row r="45" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E45" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="F45" s="23" t="s">
+      <c r="F45" s="12" t="s">
         <v>347</v>
       </c>
     </row>
@@ -6257,34 +6633,34 @@
       <c r="D46" t="s">
         <v>169</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" t="s">
         <v>357</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F46" t="s">
         <v>337</v>
       </c>
-      <c r="G46" s="15" t="s">
+      <c r="G46" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="H46" s="14" t="s">
+      <c r="H46" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="I46" s="13" t="s">
+      <c r="I46" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="J46" s="13" t="s">
+      <c r="J46" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="K46" s="14" t="s">
+      <c r="K46" s="3" t="s">
         <v>632</v>
       </c>
-      <c r="L46" s="14" t="s">
+      <c r="L46" s="3" t="s">
         <v>633</v>
       </c>
-      <c r="M46" s="13" t="s">
+      <c r="M46" s="2" t="s">
         <v>634</v>
       </c>
-      <c r="N46" s="12" t="s">
+      <c r="N46" t="s">
         <v>264</v>
       </c>
       <c r="P46" s="3" t="s">
@@ -6309,11 +6685,11 @@
         <v>640</v>
       </c>
     </row>
-    <row r="47" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E47" s="18" t="s">
+    <row r="47" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E47" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="F47" s="22" t="s">
+      <c r="F47" s="11" t="s">
         <v>360</v>
       </c>
     </row>
@@ -6330,34 +6706,34 @@
       <c r="D48" t="s">
         <v>169</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E48" t="s">
         <v>357</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F48" t="s">
         <v>266</v>
       </c>
-      <c r="G48" s="13" t="s">
+      <c r="G48" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="H48" s="14" t="s">
+      <c r="H48" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="I48" s="13" t="s">
+      <c r="I48" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="J48" s="13" t="s">
+      <c r="J48" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="K48" s="14" t="s">
+      <c r="K48" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="L48" s="14" t="s">
+      <c r="L48" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="M48" s="13" t="s">
+      <c r="M48" s="2" t="s">
         <v>644</v>
       </c>
-      <c r="N48" s="13" t="s">
+      <c r="N48" s="2" t="s">
         <v>645</v>
       </c>
       <c r="P48" s="2" t="s">
@@ -6382,12 +6758,1662 @@
         <v>651</v>
       </c>
     </row>
-    <row r="49" spans="5:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="E49" s="18" t="s">
+    <row r="49" spans="5:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E49" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="F49" s="22" t="s">
+      <c r="F49" s="11" t="s">
         <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722BC16C-B4F2-304F-A2C1-6425566A78FD}">
+  <dimension ref="A1:S149"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="135" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F141" sqref="F141"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>653</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="L2" t="s">
+        <v>658</v>
+      </c>
+      <c r="M2" t="s">
+        <v>659</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="R2" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>653</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>676</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>512</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>677</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>678</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>679</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>680</v>
+      </c>
+      <c r="O11" s="15" t="s">
+        <v>681</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>682</v>
+      </c>
+      <c r="Q11" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="R11" s="13" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>653</v>
+      </c>
+      <c r="B20" t="s">
+        <v>308</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="J20" t="s">
+        <v>689</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="L20" t="s">
+        <v>206</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="R20" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>222</v>
+      </c>
+      <c r="E22" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>223</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>224</v>
+      </c>
+      <c r="E24" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>225</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="S25" s="3"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>226</v>
+      </c>
+      <c r="E28" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>227</v>
+      </c>
+      <c r="E29" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>228</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>229</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>230</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>231</v>
+      </c>
+      <c r="E34" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>232</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>233</v>
+      </c>
+      <c r="E36" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>234</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>235</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>236</v>
+      </c>
+      <c r="E41" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>237</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>238</v>
+      </c>
+      <c r="E43" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>97</v>
+      </c>
+      <c r="E45" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>239</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>240</v>
+      </c>
+      <c r="E47" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="48" spans="4:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D48" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>653</v>
+      </c>
+      <c r="B49" t="s">
+        <v>308</v>
+      </c>
+      <c r="C49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>702</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>703</v>
+      </c>
+      <c r="I49" s="16" t="s">
+        <v>704</v>
+      </c>
+      <c r="J49" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="K49" s="16" t="s">
+        <v>705</v>
+      </c>
+      <c r="L49" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="M49" s="15" t="s">
+        <v>706</v>
+      </c>
+      <c r="N49" s="16" t="s">
+        <v>707</v>
+      </c>
+      <c r="O49" s="15" t="s">
+        <v>708</v>
+      </c>
+      <c r="P49" s="16" t="s">
+        <v>709</v>
+      </c>
+      <c r="Q49" s="15" t="s">
+        <v>710</v>
+      </c>
+      <c r="R49" s="13" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>90</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>222</v>
+      </c>
+      <c r="E51" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>223</v>
+      </c>
+      <c r="E52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>224</v>
+      </c>
+      <c r="E53" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>225</v>
+      </c>
+      <c r="E54" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E55" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>92</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>226</v>
+      </c>
+      <c r="E57" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>227</v>
+      </c>
+      <c r="E58" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>93</v>
+      </c>
+      <c r="E59" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>228</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>229</v>
+      </c>
+      <c r="E61" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>230</v>
+      </c>
+      <c r="E62" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>231</v>
+      </c>
+      <c r="E63" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
+        <v>232</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>233</v>
+      </c>
+      <c r="E65" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>234</v>
+      </c>
+      <c r="E66" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>94</v>
+      </c>
+      <c r="E67" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>235</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>95</v>
+      </c>
+      <c r="E69" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>236</v>
+      </c>
+      <c r="E70" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>237</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>238</v>
+      </c>
+      <c r="E72" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>96</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
+        <v>97</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D75" t="s">
+        <v>239</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>240</v>
+      </c>
+      <c r="E76" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D77" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="E77" s="12" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>712</v>
+      </c>
+      <c r="B78" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" t="s">
+        <v>23</v>
+      </c>
+      <c r="D78" t="s">
+        <v>44</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="K78" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="L78" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="M78" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="N78" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="O78" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="P78" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>724</v>
+      </c>
+      <c r="R78" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D79" t="s">
+        <v>91</v>
+      </c>
+      <c r="E79" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D80" t="s">
+        <v>93</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D81" t="s">
+        <v>94</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>95</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D83" t="s">
+        <v>96</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D84" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>712</v>
+      </c>
+      <c r="B85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C85" t="s">
+        <v>59</v>
+      </c>
+      <c r="D85" t="s">
+        <v>44</v>
+      </c>
+      <c r="E85" t="s">
+        <v>294</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="J85" t="s">
+        <v>730</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="L85" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="M85" t="s">
+        <v>733</v>
+      </c>
+      <c r="N85" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="O85" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="P85" t="s">
+        <v>736</v>
+      </c>
+      <c r="Q85" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="R85" s="2" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
+        <v>91</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D87" t="s">
+        <v>93</v>
+      </c>
+      <c r="E87" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
+        <v>94</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
+        <v>95</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
+        <v>96</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D91" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>712</v>
+      </c>
+      <c r="B92" t="s">
+        <v>308</v>
+      </c>
+      <c r="C92" t="s">
+        <v>23</v>
+      </c>
+      <c r="D92" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E92" s="16" t="s">
+        <v>759</v>
+      </c>
+      <c r="F92" s="16" t="s">
+        <v>685</v>
+      </c>
+      <c r="G92" s="15" t="s">
+        <v>686</v>
+      </c>
+      <c r="H92" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="I92" s="16" t="s">
+        <v>750</v>
+      </c>
+      <c r="J92" s="13" t="s">
+        <v>689</v>
+      </c>
+      <c r="K92" s="16" t="s">
+        <v>690</v>
+      </c>
+      <c r="L92" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="M92" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="N92" s="16" t="s">
+        <v>691</v>
+      </c>
+      <c r="O92" s="15" t="s">
+        <v>692</v>
+      </c>
+      <c r="P92" s="16" t="s">
+        <v>752</v>
+      </c>
+      <c r="Q92" s="16" t="s">
+        <v>693</v>
+      </c>
+      <c r="R92" s="13" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>90</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>222</v>
+      </c>
+      <c r="E94" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
+        <v>223</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
+        <v>224</v>
+      </c>
+      <c r="E96" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="97" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
+        <v>225</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="98" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>91</v>
+      </c>
+      <c r="E98" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="99" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
+        <v>92</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="100" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
+        <v>226</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="101" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D101" t="s">
+        <v>227</v>
+      </c>
+      <c r="E101" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="102" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D102" t="s">
+        <v>93</v>
+      </c>
+      <c r="E102" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="103" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D103" t="s">
+        <v>228</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="104" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D104" t="s">
+        <v>229</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="105" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D105" t="s">
+        <v>230</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="106" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D106" t="s">
+        <v>231</v>
+      </c>
+      <c r="E106" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="107" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D107" t="s">
+        <v>232</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="108" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D108" t="s">
+        <v>233</v>
+      </c>
+      <c r="E108" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="109" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D109" t="s">
+        <v>234</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="110" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D110" t="s">
+        <v>94</v>
+      </c>
+      <c r="E110" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="111" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D111" t="s">
+        <v>235</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="112" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D112" t="s">
+        <v>95</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="113" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D113" t="s">
+        <v>236</v>
+      </c>
+      <c r="E113" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="114" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
+        <v>237</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="115" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D115" t="s">
+        <v>238</v>
+      </c>
+      <c r="E115" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="116" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D116" t="s">
+        <v>96</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="117" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D117" t="s">
+        <v>97</v>
+      </c>
+      <c r="E117" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="118" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D118" t="s">
+        <v>239</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="119" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D119" t="s">
+        <v>240</v>
+      </c>
+      <c r="E119" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="120" spans="4:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D120" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="E120" s="12" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="121" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D121" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E121" t="s">
+        <v>266</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="H121" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="I121" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="J121" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="K121" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="L121" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="M121" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="N121" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="O121" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="P121" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="Q121" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="R121" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="122" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D122" t="s">
+        <v>90</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="123" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D123" t="s">
+        <v>222</v>
+      </c>
+      <c r="E123" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="124" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D124" t="s">
+        <v>223</v>
+      </c>
+      <c r="E124" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="125" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D125" t="s">
+        <v>224</v>
+      </c>
+      <c r="E125" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="126" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D126" t="s">
+        <v>225</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="127" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D127" t="s">
+        <v>91</v>
+      </c>
+      <c r="E127" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="128" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D128" t="s">
+        <v>92</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="129" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D129" t="s">
+        <v>226</v>
+      </c>
+      <c r="E129" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="130" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D130" t="s">
+        <v>227</v>
+      </c>
+      <c r="E130" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="131" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D131" t="s">
+        <v>93</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="132" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D132" t="s">
+        <v>228</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="133" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D133" t="s">
+        <v>229</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="134" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D134" t="s">
+        <v>230</v>
+      </c>
+      <c r="E134" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="135" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D135" t="s">
+        <v>231</v>
+      </c>
+      <c r="E135" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="136" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D136" t="s">
+        <v>232</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="137" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D137" t="s">
+        <v>233</v>
+      </c>
+      <c r="E137" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="138" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D138" t="s">
+        <v>234</v>
+      </c>
+      <c r="E138" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="139" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D139" t="s">
+        <v>94</v>
+      </c>
+      <c r="E139" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="140" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
+        <v>235</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="141" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D141" t="s">
+        <v>95</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="142" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D142" t="s">
+        <v>236</v>
+      </c>
+      <c r="E142" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="143" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D143" t="s">
+        <v>237</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="144" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D144" t="s">
+        <v>238</v>
+      </c>
+      <c r="E144" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="145" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D145" t="s">
+        <v>96</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="146" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D146" t="s">
+        <v>97</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="147" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D147" t="s">
+        <v>239</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="148" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D148" t="s">
+        <v>240</v>
+      </c>
+      <c r="E148" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="149" spans="4:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D149" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="E149" s="12" t="s">
+        <v>778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created forest plots for main math and RLA models
</commit_message>
<xml_diff>
--- a/tables/Model Parameters.xlsx
+++ b/tables/Model Parameters.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriellameltzer/Git/tropical_cyclones_educational_attainment_2022/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CE9184-A098-924F-A29E-376B752F58E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCCED54-A012-DD4B-918B-C0C0D97426AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15140" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="2" xr2:uid="{09DAD223-5B37-144B-8D79-2569A973BF72}"/>
+    <workbookView xWindow="11640" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="3" xr2:uid="{09DAD223-5B37-144B-8D79-2569A973BF72}"/>
   </bookViews>
   <sheets>
     <sheet name="No EM" sheetId="1" r:id="rId1"/>
     <sheet name="EM Models" sheetId="2" r:id="rId2"/>
     <sheet name="Revised" sheetId="3" r:id="rId3"/>
+    <sheet name="Revised_2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="793">
   <si>
     <t>Storm Type</t>
   </si>
@@ -2375,6 +2376,48 @@
   </si>
   <si>
     <t>0.15 (0.08, 0.22)</t>
+  </si>
+  <si>
+    <t>-0.49 (-0.86, -0.13)</t>
+  </si>
+  <si>
+    <t>1.60 (1.17, 2.02)</t>
+  </si>
+  <si>
+    <t>-0.01 (-0.04, 0.02)</t>
+  </si>
+  <si>
+    <t>-0.62 (-0.84, -0.40)</t>
+  </si>
+  <si>
+    <t>-0.30 (-0.33, -0.26)</t>
+  </si>
+  <si>
+    <t>1.63 (1.47, 1.80)</t>
+  </si>
+  <si>
+    <t>-0.70 (-0.84, -0.56)</t>
+  </si>
+  <si>
+    <t>0.08 (-0.07, 0.23)</t>
+  </si>
+  <si>
+    <t>1.43 (1.06, 1.79)</t>
+  </si>
+  <si>
+    <t>-1.51 (-1.59, -1.42)</t>
+  </si>
+  <si>
+    <t>0.05 (0.03, 0.08)</t>
+  </si>
+  <si>
+    <t>1.78 (1.64, 1.92)</t>
+  </si>
+  <si>
+    <t>-0.30 (-0.42, -0.19)</t>
+  </si>
+  <si>
+    <t>0.10 (-0.03, 0.22)</t>
   </si>
 </sst>
 </file>
@@ -2452,7 +2495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
@@ -2466,13 +2509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6775,9 +6812,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722BC16C-B4F2-304F-A2C1-6425566A78FD}">
   <dimension ref="A1:S149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="135" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F141" sqref="F141"/>
+    <sheetView zoomScale="135" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6989,46 +7026,46 @@
       <c r="D11" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" t="s">
         <v>242</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J11" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="K11" s="2" t="s">
         <v>677</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="3" t="s">
         <v>678</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="N11" s="16" t="s">
+      <c r="N11" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="3" t="s">
         <v>681</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="P11" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="Q11" s="13" t="s">
+      <c r="Q11" t="s">
         <v>683</v>
       </c>
-      <c r="R11" s="13" t="s">
+      <c r="R11" t="s">
         <v>684</v>
       </c>
     </row>
@@ -7036,7 +7073,7 @@
       <c r="D12" t="s">
         <v>90</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" t="s">
         <v>107</v>
       </c>
     </row>
@@ -7088,11 +7125,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="18" t="s">
+    <row r="19" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="11" t="s">
         <v>115</v>
       </c>
     </row>
@@ -7387,49 +7424,49 @@
       <c r="C49" t="s">
         <v>59</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" t="s">
         <v>44</v>
       </c>
-      <c r="E49" s="13" t="s">
+      <c r="E49" t="s">
         <v>299</v>
       </c>
-      <c r="F49" s="16" t="s">
+      <c r="F49" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="G49" s="15" t="s">
+      <c r="G49" s="3" t="s">
         <v>702</v>
       </c>
-      <c r="H49" s="16" t="s">
+      <c r="H49" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="I49" s="16" t="s">
+      <c r="I49" s="2" t="s">
         <v>704</v>
       </c>
-      <c r="J49" s="15" t="s">
+      <c r="J49" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="K49" s="16" t="s">
+      <c r="K49" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="L49" s="14" t="s">
+      <c r="L49" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="M49" s="15" t="s">
+      <c r="M49" s="3" t="s">
         <v>706</v>
       </c>
-      <c r="N49" s="16" t="s">
+      <c r="N49" s="2" t="s">
         <v>707</v>
       </c>
-      <c r="O49" s="15" t="s">
+      <c r="O49" s="3" t="s">
         <v>708</v>
       </c>
-      <c r="P49" s="16" t="s">
+      <c r="P49" s="2" t="s">
         <v>709</v>
       </c>
-      <c r="Q49" s="15" t="s">
+      <c r="Q49" s="3" t="s">
         <v>710</v>
       </c>
-      <c r="R49" s="13" t="s">
+      <c r="R49" t="s">
         <v>711</v>
       </c>
     </row>
@@ -7875,49 +7912,49 @@
       <c r="C92" t="s">
         <v>23</v>
       </c>
-      <c r="D92" s="13" t="s">
+      <c r="D92" t="s">
         <v>44</v>
       </c>
-      <c r="E92" s="16" t="s">
+      <c r="E92" s="2" t="s">
         <v>759</v>
       </c>
-      <c r="F92" s="16" t="s">
+      <c r="F92" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="G92" s="15" t="s">
+      <c r="G92" s="3" t="s">
         <v>686</v>
       </c>
-      <c r="H92" s="16" t="s">
+      <c r="H92" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="I92" s="16" t="s">
+      <c r="I92" s="2" t="s">
         <v>750</v>
       </c>
-      <c r="J92" s="13" t="s">
+      <c r="J92" t="s">
         <v>689</v>
       </c>
-      <c r="K92" s="16" t="s">
+      <c r="K92" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="L92" s="13" t="s">
+      <c r="L92" t="s">
         <v>206</v>
       </c>
-      <c r="M92" s="15" t="s">
+      <c r="M92" s="3" t="s">
         <v>751</v>
       </c>
-      <c r="N92" s="16" t="s">
+      <c r="N92" s="2" t="s">
         <v>691</v>
       </c>
-      <c r="O92" s="15" t="s">
+      <c r="O92" s="3" t="s">
         <v>692</v>
       </c>
-      <c r="P92" s="16" t="s">
+      <c r="P92" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="Q92" s="16" t="s">
+      <c r="Q92" s="2" t="s">
         <v>693</v>
       </c>
-      <c r="R92" s="13" t="s">
+      <c r="R92" t="s">
         <v>753</v>
       </c>
     </row>
@@ -8146,7 +8183,7 @@
       </c>
     </row>
     <row r="121" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D121" s="13" t="s">
+      <c r="D121" t="s">
         <v>44</v>
       </c>
       <c r="E121" t="s">
@@ -8415,6 +8452,1001 @@
       <c r="E149" s="12" t="s">
         <v>778</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A397E929-D643-0C48-99AF-0CE7A48E8A31}">
+  <dimension ref="A1:Q147"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20:D48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>653</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="L2" t="s">
+        <v>658</v>
+      </c>
+      <c r="M2" t="s">
+        <v>659</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>653</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>242</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>653</v>
+      </c>
+      <c r="B20" t="s">
+        <v>308</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="L20" t="s">
+        <v>206</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>222</v>
+      </c>
+      <c r="E22" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>223</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>224</v>
+      </c>
+      <c r="E24" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>225</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>226</v>
+      </c>
+      <c r="E28" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>227</v>
+      </c>
+      <c r="E29" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>228</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>229</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>230</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>231</v>
+      </c>
+      <c r="E34" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>232</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>233</v>
+      </c>
+      <c r="E36" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>234</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>235</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>236</v>
+      </c>
+      <c r="E41" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>237</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>238</v>
+      </c>
+      <c r="E43" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>97</v>
+      </c>
+      <c r="E45" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>239</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>240</v>
+      </c>
+      <c r="E47" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="48" spans="4:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D48" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>653</v>
+      </c>
+      <c r="B49" t="s">
+        <v>308</v>
+      </c>
+      <c r="C49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" t="s">
+        <v>299</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>90</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>222</v>
+      </c>
+      <c r="E51" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>223</v>
+      </c>
+      <c r="E52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>224</v>
+      </c>
+      <c r="E53" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>225</v>
+      </c>
+      <c r="E54" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E55" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>92</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>226</v>
+      </c>
+      <c r="E57" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>227</v>
+      </c>
+      <c r="E58" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>93</v>
+      </c>
+      <c r="E59" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>228</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>229</v>
+      </c>
+      <c r="E61" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>230</v>
+      </c>
+      <c r="E62" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>231</v>
+      </c>
+      <c r="E63" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
+        <v>232</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="65" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>233</v>
+      </c>
+      <c r="E65" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="66" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>234</v>
+      </c>
+      <c r="E66" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="67" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>94</v>
+      </c>
+      <c r="E67" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="68" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>235</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="69" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>95</v>
+      </c>
+      <c r="E69" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="70" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>236</v>
+      </c>
+      <c r="E70" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="71" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>237</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="72" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>238</v>
+      </c>
+      <c r="E72" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="73" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>96</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="74" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
+        <v>97</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="75" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D75" t="s">
+        <v>239</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="76" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>240</v>
+      </c>
+      <c r="E76" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="77" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D77" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="E77" s="12" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="78" spans="4:17" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+    </row>
+    <row r="80" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="E80" s="1"/>
+    </row>
+    <row r="81" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E82" s="1"/>
+    </row>
+    <row r="83" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E83" s="1"/>
+    </row>
+    <row r="85" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="F85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="K85" s="1"/>
+      <c r="N85" s="1"/>
+      <c r="Q85" s="1"/>
+    </row>
+    <row r="88" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E88" s="1"/>
+    </row>
+    <row r="89" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="N92" s="1"/>
+      <c r="P92" s="1"/>
+    </row>
+    <row r="93" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E93" s="1"/>
+    </row>
+    <row r="95" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E95" s="1"/>
+    </row>
+    <row r="103" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E103" s="1"/>
+    </row>
+    <row r="104" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E104" s="1"/>
+    </row>
+    <row r="105" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E105" s="1"/>
+    </row>
+    <row r="109" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E109" s="1"/>
+    </row>
+    <row r="111" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E111" s="1"/>
+    </row>
+    <row r="112" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E112" s="1"/>
+    </row>
+    <row r="114" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E114" s="1"/>
+    </row>
+    <row r="116" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E116" s="1"/>
+    </row>
+    <row r="118" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E118" s="1"/>
+    </row>
+    <row r="121" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="F121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1"/>
+      <c r="K121" s="1"/>
+      <c r="L121" s="1"/>
+      <c r="N121" s="1"/>
+      <c r="P121" s="1"/>
+    </row>
+    <row r="122" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E122" s="1"/>
+    </row>
+    <row r="132" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E132" s="1"/>
+    </row>
+    <row r="133" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E133" s="1"/>
+    </row>
+    <row r="140" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E140" s="1"/>
+    </row>
+    <row r="141" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E141" s="1"/>
+    </row>
+    <row r="143" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E143" s="1"/>
+    </row>
+    <row r="145" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E145" s="1"/>
+    </row>
+    <row r="146" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E146" s="1"/>
+    </row>
+    <row r="147" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E147" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
First draft of paper
</commit_message>
<xml_diff>
--- a/tables/Model Parameters.xlsx
+++ b/tables/Model Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriellameltzer/Git/tropical_cyclones_educational_attainment_2022/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCCED54-A012-DD4B-918B-C0C0D97426AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D7F208-27A0-6A43-B530-11CDCC1DBC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="3" xr2:uid="{09DAD223-5B37-144B-8D79-2569A973BF72}"/>
+    <workbookView xWindow="11920" yWindow="520" windowWidth="28800" windowHeight="16240" activeTab="3" xr2:uid="{09DAD223-5B37-144B-8D79-2569A973BF72}"/>
   </bookViews>
   <sheets>
     <sheet name="No EM" sheetId="1" r:id="rId1"/>
@@ -8463,7 +8463,7 @@
   <dimension ref="A1:Q147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:D48"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>